<commit_message>
update plan 20201112 & update result 20201111
</commit_message>
<xml_diff>
--- a/20201111.xlsx
+++ b/20201111.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD600C8-5590-4597-AF55-49D859C8A0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7FCB1B-23C3-4518-AE56-122899B5C77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>일</t>
   </si>
@@ -153,10 +154,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>많은 자극을 받는 행동을 자제하자</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">7:30 ~ 8:10 </t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -215,6 +212,31 @@
   </si>
   <si>
     <t>어둠 코딩(1시간)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>일일업무</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>자극을 많이 받는행동을 자제하자</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>F7 부분공용
+ - 충전완료 화면에서 CP가 12v가 될 시에, disconnect화면으로 넘어가도록 변경
+  -&gt; 기존 태그까지 무한 대기하던 현상 수정
+ - 충전내역 로그에서 넘버링이 F7이 재부팅할 시 초기화 되던 현상 수정
+  -&gt; 초기 부팅 시 충전내역 로그를 한번 읽고, 마지막 충전 넘버링을 계산하도록 변경
+ - 충전중 EMG발생 시 충전종료(35번전문) 전송
+  -&gt; 충전중 비상정지 버튼 누를 시, fault화면 진입과 동시에 35번전문 서버로 전송
+2채널
+ - 80도에 에러발생, 75도 미만일 경우 해제 및 소스코드 전달(김철호 부사장님)
+  -&gt; IOC파일의 ADC쪽 에러 수정 (72MHZ사용할 경우 ADC freescale사용 해야 함.)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>술먹음</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -388,7 +410,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,8 +627,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -723,63 +757,11 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -825,43 +807,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -997,116 +942,119 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1639,10 +1587,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:L25"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E23" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1651,329 +1599,384 @@
     <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.125" customWidth="1"/>
     <col min="6" max="6" width="85.75" customWidth="1"/>
-    <col min="8" max="8" width="39.75" customWidth="1"/>
-    <col min="10" max="10" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="78" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="39.75" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1"/>
+    <col min="12" max="12" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="23"/>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="23"/>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="23"/>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="23"/>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <f>SUM(J3:J6)</f>
+        <v>206</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="23"/>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="23"/>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>309</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="2:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
+      <c r="D11" s="34"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4">
+      <c r="D16" s="34"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7">
-        <f>SUM(I3:I6)</f>
-        <v>206</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="6"/>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>309</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="2:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="29" t="s">
+      <c r="D17" s="34"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="34"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="C19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C20" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
+      <c r="C21" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
+      <c r="C22" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="34"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="23"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="24" t="s">
+      <c r="C23" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="D23" s="35"/>
+      <c r="E23" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="28"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="G3:G24"/>
     <mergeCell ref="F3:F24"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E23:E24"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>